<commit_message>
code cleanup initial commit
</commit_message>
<xml_diff>
--- a/data/input/seaworld/seaworld_api_data.xlsx
+++ b/data/input/seaworld/seaworld_api_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pednsid\Code\code\web_scraping_projects\amusement_park_scrape\data\input\seaworld\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00B824DD-919D-4884-AC06-EC3435E6D4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8925C30C-6768-4984-9FAA-F614FB9FE917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BA79B024-9B49-40D5-9AB8-CE64A07467BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Company</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>https://sesameplace.com/api/sitecore/CalendarEvents/LoadCalendarData?itemId=5a890592-5e34-420c-a491-0a0d0c8f2695</t>
+  </si>
+  <si>
+    <t>https://seaworld.com/api/sitecore/CalendarEvents/LoadCalendarData?itemId=01d7932a-e537-476b-b658-e3e4b7f6677f</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -533,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAAF07E-5793-4CEF-AF4C-87D6CF08B368}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,7 +573,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -716,27 +719,27 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{53BEBAFD-F0A3-44AA-9C21-D07633574112}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{1D9EC4C7-2577-44F6-9A7B-3DC109A4087F}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{4AB7C373-3488-42B0-95F6-1900788A5C3D}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{478A21A8-7D4F-4732-937A-1E5E36B29471}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{7F31E621-FE8B-4DCD-995D-93EA9CCDD01C}"/>
-    <hyperlink ref="D4" r:id="rId6" xr:uid="{A31C30F9-C332-424F-A826-554DED5CA7B4}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{FDF2E549-94A5-40ED-B46C-752BCF0B3252}"/>
-    <hyperlink ref="D5" r:id="rId8" xr:uid="{38A20293-CBC5-4660-80DD-BF1B92AB03BF}"/>
-    <hyperlink ref="C6" r:id="rId9" xr:uid="{AB6D2465-CA3B-44F2-B088-6641FB4A4CFC}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{4DA14FD8-1705-4724-9211-FA4771B67589}"/>
-    <hyperlink ref="C7" r:id="rId11" xr:uid="{86786653-75B8-4DF3-ABE8-4DE5C1082CF3}"/>
-    <hyperlink ref="D7" r:id="rId12" xr:uid="{62D0E831-5214-4CFC-991E-1D3C75B4724E}"/>
-    <hyperlink ref="C8" r:id="rId13" xr:uid="{AD772E37-E91A-4621-952C-FCBF3BDCA7B6}"/>
-    <hyperlink ref="D8" r:id="rId14" xr:uid="{278D9756-D388-4B62-950F-1F1C58AA163B}"/>
-    <hyperlink ref="C9" r:id="rId15" xr:uid="{8ABFF8F5-899D-4F1C-94A0-73545FF5DD0A}"/>
-    <hyperlink ref="D9" r:id="rId16" xr:uid="{8063C496-C26F-49EB-AAAF-D3E38A5AAFD3}"/>
-    <hyperlink ref="C10" r:id="rId17" xr:uid="{6D7041C6-B621-4BB4-AD2F-D5781B5A7FE8}"/>
-    <hyperlink ref="D10" r:id="rId18" xr:uid="{175B6AC1-F4CF-41FA-89AC-257214C5E3C8}"/>
-    <hyperlink ref="C11" r:id="rId19" xr:uid="{07C1736B-78A9-451B-BE05-7E5DD494DFF2}"/>
-    <hyperlink ref="D11" r:id="rId20" xr:uid="{15C1EA74-6C95-4F61-A2CA-9A23CD610D97}"/>
-    <hyperlink ref="C12" r:id="rId21" xr:uid="{A98A192D-EBCA-4C24-8881-AB4995D47D18}"/>
-    <hyperlink ref="D12" r:id="rId22" xr:uid="{54D8F7FE-C275-4859-AAA0-840C87772283}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{4AB7C373-3488-42B0-95F6-1900788A5C3D}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{478A21A8-7D4F-4732-937A-1E5E36B29471}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{7F31E621-FE8B-4DCD-995D-93EA9CCDD01C}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{A31C30F9-C332-424F-A826-554DED5CA7B4}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{FDF2E549-94A5-40ED-B46C-752BCF0B3252}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{38A20293-CBC5-4660-80DD-BF1B92AB03BF}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{AB6D2465-CA3B-44F2-B088-6641FB4A4CFC}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{4DA14FD8-1705-4724-9211-FA4771B67589}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{86786653-75B8-4DF3-ABE8-4DE5C1082CF3}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{62D0E831-5214-4CFC-991E-1D3C75B4724E}"/>
+    <hyperlink ref="C8" r:id="rId12" xr:uid="{AD772E37-E91A-4621-952C-FCBF3BDCA7B6}"/>
+    <hyperlink ref="D8" r:id="rId13" xr:uid="{278D9756-D388-4B62-950F-1F1C58AA163B}"/>
+    <hyperlink ref="C9" r:id="rId14" xr:uid="{8ABFF8F5-899D-4F1C-94A0-73545FF5DD0A}"/>
+    <hyperlink ref="D9" r:id="rId15" xr:uid="{8063C496-C26F-49EB-AAAF-D3E38A5AAFD3}"/>
+    <hyperlink ref="C10" r:id="rId16" xr:uid="{6D7041C6-B621-4BB4-AD2F-D5781B5A7FE8}"/>
+    <hyperlink ref="D10" r:id="rId17" xr:uid="{175B6AC1-F4CF-41FA-89AC-257214C5E3C8}"/>
+    <hyperlink ref="C11" r:id="rId18" xr:uid="{07C1736B-78A9-451B-BE05-7E5DD494DFF2}"/>
+    <hyperlink ref="D11" r:id="rId19" xr:uid="{15C1EA74-6C95-4F61-A2CA-9A23CD610D97}"/>
+    <hyperlink ref="C12" r:id="rId20" xr:uid="{A98A192D-EBCA-4C24-8881-AB4995D47D18}"/>
+    <hyperlink ref="D12" r:id="rId21" xr:uid="{54D8F7FE-C275-4859-AAA0-840C87772283}"/>
+    <hyperlink ref="D2" r:id="rId22" xr:uid="{ABF43210-E9FC-42CC-8F90-FE8A78E41236}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>